<commit_message>
[IDP-51] Activated autoscaling with target CPU usage to 70%
</commit_message>
<xml_diff>
--- a/src/test/resources/group/invalid_format.xlsx
+++ b/src/test/resources/group/invalid_format.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sterragn\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\madilisa\Desktop\ws\idpay-group\src\test\resources\group\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{846539A7-3557-4172-8219-E61DA3C6711B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFE1CE7F-3328-4959-A25E-6FBE813D9E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1725" yWindow="1035" windowWidth="26565" windowHeight="14160"/>
+    <workbookView xWindow="2580" yWindow="1968" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ps_fiscal_code_groups_file_larg" sheetId="1" r:id="rId1"/>
@@ -19,73 +19,8 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
-  <si>
-    <t>AOISFN73R54B745Z</t>
-  </si>
-  <si>
-    <t>BAAHMD77P30Z330S</t>
-  </si>
-  <si>
-    <t>BAAMRO82C23Z330C</t>
-  </si>
-  <si>
-    <t>BAEBNR90E20Z216W</t>
-  </si>
-  <si>
-    <t>BAEKKK44D42Z219I</t>
-  </si>
-  <si>
-    <t>BAEKSR79L06Z249S</t>
-  </si>
-  <si>
-    <t>BAEMRD84E66Z216B</t>
-  </si>
-  <si>
-    <t>BAICLD60M12F205M</t>
-  </si>
-  <si>
-    <t>BAICLD79L54A089Y</t>
-  </si>
-  <si>
-    <t>BAICNH82A02Z210D</t>
-  </si>
-  <si>
-    <t>BAICNL90L30Z129Z</t>
-  </si>
-  <si>
-    <t>BAICRI60R13F839M</t>
-  </si>
-  <si>
-    <t>BAIDNL73C60E202V</t>
-  </si>
-  <si>
-    <t>BAIGNE51S23F465N</t>
-  </si>
-  <si>
-    <t>BAIGPP69L63A064W</t>
-  </si>
-  <si>
-    <t>BAIGRG96R70H501Y</t>
-  </si>
-  <si>
-    <t>BAIHNN88T51Z330L</t>
-  </si>
-  <si>
-    <t>BAIHSN70S23Z352B</t>
-  </si>
-  <si>
-    <t>BAILRA61S60I625H</t>
-  </si>
-  <si>
-    <t>BAIMLB77D52F912F</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -567,48 +502,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="20% - Colore 1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Colore 2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Colore 3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Colore 4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Colore 5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Colore 6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Colore 1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Colore 2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Colore 3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Colore 4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Colore 5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Colore 6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Colore 1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Colore 2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Colore 3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Colore 4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Colore 5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Colore 6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Calcolo" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Cella collegata" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Cella da controllare" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Colore 1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Colore 2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Colore 3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Colore 4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Colore 5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Colore 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Neutrale" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Nota" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Testo avviso" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Testo descrittivo" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Titolo" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Titolo 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Titolo 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Titolo 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Titolo 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Totale" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Valore non valido" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Valore valido" xfId="6" builtinId="26" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -624,7 +559,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -912,121 +847,23 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>